<commit_message>
Fixed typo "Indutries" in Data/Mappings.
</commit_message>
<xml_diff>
--- a/Data/Mappings/BC CESI Mapping.xlsx
+++ b/Data/Mappings/BC CESI Mapping.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flerovskyg\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FlerovskyG\Desktop\CESI-Air-Pollutants\Data\Mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="0" windowWidth="23040" windowHeight="9150"/>
+    <workbookView xWindow="4575" yWindow="0" windowWidth="23040" windowHeight="9150"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -104,9 +104,6 @@
     <t>Manufacturing | Wood Products</t>
   </si>
   <si>
-    <t>Ore and mineral indutries</t>
-  </si>
-  <si>
     <t>Column1</t>
   </si>
   <si>
@@ -177,6 +174,9 @@
   </si>
   <si>
     <t>Oil and Gas Industry | Downstream Oil and Gas Industry | Natural Gas Distribution</t>
+  </si>
+  <si>
+    <t>Ore and mineral industries</t>
   </si>
 </sst>
 </file>
@@ -656,18 +656,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="B2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -720,46 +720,46 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -770,7 +770,7 @@
         <v>22</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -781,12 +781,12 @@
         <v>22</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
@@ -794,7 +794,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
@@ -802,7 +802,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" t="s">
         <v>14</v>
@@ -810,7 +810,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" t="s">
         <v>14</v>
@@ -818,7 +818,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
         <v>14</v>
@@ -826,7 +826,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
         <v>14</v>
@@ -834,7 +834,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
         <v>14</v>
@@ -842,7 +842,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22" t="s">
         <v>14</v>
@@ -850,7 +850,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
         <v>14</v>
@@ -858,7 +858,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
         <v>14</v>
@@ -866,7 +866,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B25" t="s">
         <v>14</v>
@@ -874,7 +874,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B26" t="s">
         <v>14</v>
@@ -882,46 +882,46 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>